<commit_message>
analysis script for laws network
</commit_message>
<xml_diff>
--- a/scripts/laws-influences.xlsx
+++ b/scripts/laws-influences.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/repos/law-networks-v2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/repos/imperial-networks/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="197">
   <si>
     <t>Name of the Law</t>
   </si>
@@ -1672,9 +1672,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="92" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3279,6 +3279,9 @@
       <c r="I46" s="2">
         <v>69</v>
       </c>
+      <c r="J46" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="K46" s="2" t="s">
         <v>131</v>
       </c>
@@ -3345,6 +3348,9 @@
       </c>
       <c r="I48" s="2">
         <v>53</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="K48" s="7" t="s">
         <v>135</v>

</xml_diff>